<commit_message>
[upgrade]: handle todo, cmp it -> succ ;
</commit_message>
<xml_diff>
--- a/data/data_17_12_24.xlsx
+++ b/data/data_17_12_24.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinh/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinh/code/Calendar_UTC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478FFAA7-2436-6947-B677-E25565E84A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EDAB0D-E08C-B74D-9016-C0CFC5AC9944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4280" yWindow="820" windowWidth="25960" windowHeight="17440" xr2:uid="{8E2B0296-D0D8-664E-A731-D4BACB3512B1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="40">
   <si>
     <t>Lớp học phần</t>
   </si>
@@ -240,18 +240,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -260,8 +251,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,10 +577,17 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:E26"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="43.1640625" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="27.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -602,406 +606,429 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="65" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:5" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="39" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="C15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="4" t="s">
+      <c r="A18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="C18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="C19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4" t="s">
+    <row r="20" spans="1:5" ht="39" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="4" t="s">
+      <c r="C20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="4" t="s">
+    <row r="21" spans="1:5" ht="39" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="C21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="4" t="s">
+      <c r="C22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4" t="s">
+    <row r="23" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4" t="s">
+    <row r="24" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="C24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="4" t="s">
+      <c r="A25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="4" t="s">
+      <c r="C25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="52" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
+    <row r="26" spans="1:5" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="4" t="s">
+      <c r="C26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="4">
     <mergeCell ref="E23:E24"/>
-    <mergeCell ref="A22:A25"/>
     <mergeCell ref="E16:E17"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A13:A14"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[uprade]: cmp format new xml and data json new
</commit_message>
<xml_diff>
--- a/data/data_17_12_24.xlsx
+++ b/data/data_17_12_24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinh/code/Calendar_UTC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EDAB0D-E08C-B74D-9016-C0CFC5AC9944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10139AF4-EE34-1B4F-831A-4F0EEA410AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4280" yWindow="820" windowWidth="25960" windowHeight="17440" xr2:uid="{8E2B0296-D0D8-664E-A731-D4BACB3512B1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="40">
   <si>
     <t>Lớp học phần</t>
   </si>
@@ -240,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -252,9 +252,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -577,7 +574,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,7 +604,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -623,8 +620,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -657,8 +654,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -674,8 +671,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -691,8 +688,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -709,7 +706,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -726,7 +723,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -738,10 +735,12 @@
       <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -758,7 +757,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -770,7 +769,9 @@
       <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -789,8 +790,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -806,8 +807,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -823,8 +824,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -840,8 +841,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -857,8 +858,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -870,10 +871,12 @@
       <c r="D17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="E17" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -890,7 +893,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -906,8 +909,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="39" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -923,8 +926,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="39" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -940,8 +943,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -957,8 +960,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -974,8 +977,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -987,10 +990,12 @@
       <c r="D24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" ht="26" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+      <c r="E24" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1024,12 +1029,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E11"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[upgrade]: fix data new
</commit_message>
<xml_diff>
--- a/data/data_17_12_24.xlsx
+++ b/data/data_17_12_24.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinh/code/Calendar_UTC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10139AF4-EE34-1B4F-831A-4F0EEA410AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4904479C-2416-7547-AC6E-F2A4314FAABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="820" windowWidth="25960" windowHeight="17440" xr2:uid="{8E2B0296-D0D8-664E-A731-D4BACB3512B1}"/>
+    <workbookView xWindow="4280" yWindow="820" windowWidth="25960" windowHeight="17440" activeTab="1" xr2:uid="{8E2B0296-D0D8-664E-A731-D4BACB3512B1}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="data2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="42">
   <si>
     <t>Lớp học phần</t>
   </si>
@@ -155,13 +156,19 @@
   </si>
   <si>
     <t>Trí thuệ nhân tạo-1-2-24(QT(TA)01.BT1)</t>
+  </si>
+  <si>
+    <t>Lập trình thiết bị di động-1-2-24(QT(TA)02.BT1)</t>
+  </si>
+  <si>
+    <t>Lập trình thiết bị di động-1-2-24(QT(TA)02)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -177,6 +184,12 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -240,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -255,6 +268,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -573,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{325CFBBD-3CDA-1B40-BA4C-173D2FA00E1A}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1031,4 +1050,121 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8E51B63-3648-704F-8EED-BEEED70C31DB}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="6" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+      <c r="A3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+      <c r="A5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
+      <c r="A6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>